<commit_message>
last changes and readme file
</commit_message>
<xml_diff>
--- a/data/2014.xlsx
+++ b/data/2014.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dev\Desktop\DSPT2025\2-Data Analysis\Proyecto final de módulo\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dev\Desktop\EuroElection-Trends\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C810475-4640-4029-BBAE-3B12E2E23827}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A017C41A-9BCC-41B5-97AC-233BBD7CA547}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14616" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="768" yWindow="768" windowWidth="19356" windowHeight="11808" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Provincias" sheetId="1" r:id="rId1"/>
@@ -400,9 +400,6 @@
     <t>MOVIMIENTO CORRIENTE ROJA</t>
   </si>
   <si>
-    <t>P.P.</t>
-  </si>
-  <si>
     <t>PSOE</t>
   </si>
   <si>
@@ -416,9 +413,6 @@
   </si>
   <si>
     <t>EPDD</t>
-  </si>
-  <si>
-    <t>C's</t>
   </si>
   <si>
     <t>LPD</t>
@@ -439,19 +433,10 @@
     <t>PIRATAS</t>
   </si>
   <si>
-    <t>F.A.C.</t>
-  </si>
-  <si>
     <t>DISCAPACITADOS Y ENFERMEDADES RARAS</t>
   </si>
   <si>
     <t>RECORTES CERO</t>
-  </si>
-  <si>
-    <t>P.C.P.E.</t>
-  </si>
-  <si>
-    <t>I.Fem</t>
   </si>
   <si>
     <t>FE de las JONS</t>
@@ -469,19 +454,10 @@
     <t>PH</t>
   </si>
   <si>
-    <t>D.N.</t>
-  </si>
-  <si>
     <t>ACNV-BAR-PRAO-R.E.P.O-UNIO</t>
   </si>
   <si>
     <t>PT</t>
-  </si>
-  <si>
-    <t>P-LIB</t>
-  </si>
-  <si>
-    <t>M.S.R.</t>
   </si>
   <si>
     <t>ALTER</t>
@@ -499,13 +475,37 @@
     <t>IPEX-PREX-CREX</t>
   </si>
   <si>
-    <t>M.C.R.</t>
-  </si>
-  <si>
     <t>Total</t>
   </si>
   <si>
     <t xml:space="preserve">IZQUIERDA UNIDA </t>
+  </si>
+  <si>
+    <t>PP</t>
+  </si>
+  <si>
+    <t>MSR</t>
+  </si>
+  <si>
+    <t>DN</t>
+  </si>
+  <si>
+    <t>PCPE</t>
+  </si>
+  <si>
+    <t>FAC</t>
+  </si>
+  <si>
+    <t>IFem</t>
+  </si>
+  <si>
+    <t>CS</t>
+  </si>
+  <si>
+    <t>MCR</t>
+  </si>
+  <si>
+    <t>PLIB</t>
   </si>
 </sst>
 </file>
@@ -1419,8 +1419,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CP60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="Y4" sqref="Y4:Z4"/>
+    <sheetView tabSelected="1" topLeftCell="V4" workbookViewId="0">
+      <selection activeCell="BY5" sqref="BY5:BZ5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1447,7 +1447,7 @@
       </c>
       <c r="T4" s="9"/>
       <c r="U4" s="9" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="V4" s="9"/>
       <c r="W4" s="9" t="s">
@@ -1597,15 +1597,15 @@
     </row>
     <row r="5" spans="1:94" s="2" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="Q5" s="9" t="s">
-        <v>126</v>
+        <v>153</v>
       </c>
       <c r="R5" s="9"/>
       <c r="S5" s="9" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="T5" s="9"/>
       <c r="U5" s="9" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="V5" s="9"/>
       <c r="W5" s="9" t="s">
@@ -1613,23 +1613,23 @@
       </c>
       <c r="X5" s="9"/>
       <c r="Y5" s="9" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="Z5" s="9"/>
       <c r="AA5" s="9" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="AB5" s="9"/>
       <c r="AC5" s="9" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="AD5" s="9"/>
       <c r="AE5" s="9" t="s">
-        <v>132</v>
+        <v>159</v>
       </c>
       <c r="AF5" s="9"/>
       <c r="AG5" s="9" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="AH5" s="9"/>
       <c r="AI5" s="9" t="s">
@@ -1641,19 +1641,19 @@
       </c>
       <c r="AL5" s="9"/>
       <c r="AM5" s="9" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="AN5" s="9"/>
       <c r="AO5" s="9" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="AP5" s="9"/>
       <c r="AQ5" s="9" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="AR5" s="9"/>
       <c r="AS5" s="9" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="AT5" s="9"/>
       <c r="AU5" s="9" t="s">
@@ -1661,67 +1661,67 @@
       </c>
       <c r="AV5" s="9"/>
       <c r="AW5" s="9" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="AX5" s="9"/>
       <c r="AY5" s="9" t="s">
-        <v>139</v>
+        <v>157</v>
       </c>
       <c r="AZ5" s="9"/>
       <c r="BA5" s="9" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="BB5" s="9"/>
       <c r="BC5" s="9" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="BD5" s="9"/>
       <c r="BE5" s="9" t="s">
-        <v>142</v>
+        <v>156</v>
       </c>
       <c r="BF5" s="9"/>
       <c r="BG5" s="9" t="s">
-        <v>143</v>
+        <v>158</v>
       </c>
       <c r="BH5" s="9"/>
       <c r="BI5" s="9" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="BJ5" s="9"/>
       <c r="BK5" s="9" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="BL5" s="9"/>
       <c r="BM5" s="9" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="BN5" s="9"/>
       <c r="BO5" s="9" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="BP5" s="9"/>
       <c r="BQ5" s="9" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="BR5" s="9"/>
       <c r="BS5" s="9" t="s">
-        <v>149</v>
+        <v>155</v>
       </c>
       <c r="BT5" s="9"/>
       <c r="BU5" s="9" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="BV5" s="9"/>
       <c r="BW5" s="9" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="BX5" s="9"/>
       <c r="BY5" s="9" t="s">
-        <v>152</v>
+        <v>161</v>
       </c>
       <c r="BZ5" s="9"/>
       <c r="CA5" s="9" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="CB5" s="9"/>
       <c r="CC5" s="9" t="s">
@@ -1729,27 +1729,27 @@
       </c>
       <c r="CD5" s="9"/>
       <c r="CE5" s="9" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="CF5" s="9"/>
       <c r="CG5" s="9" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="CH5" s="9"/>
       <c r="CI5" s="9" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="CJ5" s="9"/>
       <c r="CK5" s="9" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="CL5" s="9"/>
       <c r="CM5" s="9" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
       <c r="CN5" s="9"/>
       <c r="CO5" s="9" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="CP5" s="9"/>
     </row>
@@ -16863,7 +16863,7 @@
       </c>
       <c r="B60" s="5"/>
       <c r="C60" s="5" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
       <c r="D60" s="7">
         <v>47129783</v>

</xml_diff>